<commit_message>
updating scripts with notes - KAR
</commit_message>
<xml_diff>
--- a/2023/field_check_match_ACnum.xlsx
+++ b/2023/field_check_match_ACnum.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nysemail-my.sharepoint.com/personal/keleigh_reynolds_dec_ny_gov/Documents/Desktop/R_SMAS/wave_data_processing/2023/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:40009_{DBFBBE73-1E41-4A82-A0D4-95843DFC9B1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5D758C51-AB5F-4C06-87E5-A89FB0E5F67A}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:40009_{DBFBBE73-1E41-4A82-A0D4-95843DFC9B1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F1D09C7F-CFB4-4DBC-B684-4A4955AF6839}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-1800" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="field_check_match_ACnum" sheetId="1" r:id="rId1"/>
@@ -2408,18 +2408,18 @@
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="27" style="4" customWidth="1"/>
-    <col min="4" max="4" width="16.5703125" customWidth="1"/>
-    <col min="5" max="5" width="18.7109375" customWidth="1"/>
-    <col min="6" max="6" width="27.42578125" style="8" customWidth="1"/>
+    <col min="4" max="4" width="16.54296875" customWidth="1"/>
+    <col min="5" max="5" width="18.7265625" customWidth="1"/>
+    <col min="6" max="6" width="27.453125" style="8" customWidth="1"/>
     <col min="7" max="7" width="30" style="8" customWidth="1"/>
-    <col min="11" max="11" width="13.42578125" customWidth="1"/>
-    <col min="37" max="37" width="19.140625" customWidth="1"/>
+    <col min="11" max="11" width="13.453125" customWidth="1"/>
+    <col min="37" max="37" width="19.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>370</v>
       </c>
@@ -2559,7 +2559,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:46" x14ac:dyDescent="0.35">
       <c r="B2">
         <v>42.441303509999997</v>
       </c>
@@ -2693,7 +2693,7 @@
         <v>42.441303509999997</v>
       </c>
     </row>
-    <row r="3" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:46" x14ac:dyDescent="0.35">
       <c r="B3">
         <v>42.520661109999999</v>
       </c>
@@ -2827,7 +2827,7 @@
         <v>42.520661109999999</v>
       </c>
     </row>
-    <row r="4" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:46" x14ac:dyDescent="0.35">
       <c r="B4">
         <v>42.875577739999997</v>
       </c>
@@ -2958,7 +2958,7 @@
         <v>42.875577739999997</v>
       </c>
     </row>
-    <row r="5" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:46" x14ac:dyDescent="0.35">
       <c r="B5">
         <v>42.451894439999997</v>
       </c>
@@ -3086,7 +3086,7 @@
         <v>42.451894439999997</v>
       </c>
     </row>
-    <row r="6" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:46" x14ac:dyDescent="0.35">
       <c r="B6">
         <v>43.084837</v>
       </c>
@@ -3217,7 +3217,7 @@
         <v>43.084837</v>
       </c>
     </row>
-    <row r="7" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:46" x14ac:dyDescent="0.35">
       <c r="B7">
         <v>43.03189252</v>
       </c>
@@ -3345,7 +3345,7 @@
         <v>43.03189252</v>
       </c>
     </row>
-    <row r="8" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:46" x14ac:dyDescent="0.35">
       <c r="B8">
         <v>42.115709109999997</v>
       </c>
@@ -3473,7 +3473,7 @@
         <v>42.115709109999997</v>
       </c>
     </row>
-    <row r="9" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:46" x14ac:dyDescent="0.35">
       <c r="B9">
         <v>43.219700000000003</v>
       </c>
@@ -3601,7 +3601,7 @@
         <v>43.219700000000003</v>
       </c>
     </row>
-    <row r="10" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:46" x14ac:dyDescent="0.35">
       <c r="B10">
         <v>43.348599999999998</v>
       </c>
@@ -3726,7 +3726,7 @@
         <v>43.348599999999998</v>
       </c>
     </row>
-    <row r="11" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:46" x14ac:dyDescent="0.35">
       <c r="B11">
         <v>43.314999999999998</v>
       </c>
@@ -3854,7 +3854,7 @@
         <v>43.314999999999998</v>
       </c>
     </row>
-    <row r="12" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:46" x14ac:dyDescent="0.35">
       <c r="B12">
         <v>42.67589358</v>
       </c>
@@ -3985,7 +3985,7 @@
         <v>42.67589358</v>
       </c>
     </row>
-    <row r="13" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:46" x14ac:dyDescent="0.35">
       <c r="B13">
         <v>42.649699810000001</v>
       </c>
@@ -4116,7 +4116,7 @@
         <v>42.649699810000001</v>
       </c>
     </row>
-    <row r="14" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:46" x14ac:dyDescent="0.35">
       <c r="B14">
         <v>42.642045340000003</v>
       </c>
@@ -4250,7 +4250,7 @@
         <v>42.642045340000003</v>
       </c>
     </row>
-    <row r="15" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:46" x14ac:dyDescent="0.35">
       <c r="B15">
         <v>43.696573999999998</v>
       </c>
@@ -4381,7 +4381,7 @@
         <v>43.696573999999998</v>
       </c>
     </row>
-    <row r="16" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:46" x14ac:dyDescent="0.35">
       <c r="B16">
         <v>43.094038980000001</v>
       </c>
@@ -4512,7 +4512,7 @@
         <v>43.094038980000001</v>
       </c>
     </row>
-    <row r="17" spans="2:46" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:46" x14ac:dyDescent="0.35">
       <c r="B17">
         <v>43.469238060000002</v>
       </c>
@@ -4640,7 +4640,7 @@
         <v>43.469238060000002</v>
       </c>
     </row>
-    <row r="18" spans="2:46" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:46" x14ac:dyDescent="0.35">
       <c r="B18">
         <v>43.229572539999999</v>
       </c>
@@ -4771,7 +4771,7 @@
         <v>43.229572539999999</v>
       </c>
     </row>
-    <row r="19" spans="2:46" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:46" x14ac:dyDescent="0.35">
       <c r="B19">
         <v>44.308059999999998</v>
       </c>
@@ -4902,7 +4902,7 @@
         <v>44.308059999999998</v>
       </c>
     </row>
-    <row r="20" spans="2:46" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:46" x14ac:dyDescent="0.35">
       <c r="B20">
         <v>43.480795110000003</v>
       </c>
@@ -5033,7 +5033,7 @@
         <v>43.480795110000003</v>
       </c>
     </row>
-    <row r="21" spans="2:46" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:46" x14ac:dyDescent="0.35">
       <c r="B21">
         <v>43.586244989999997</v>
       </c>
@@ -5164,7 +5164,7 @@
         <v>43.586244989999997</v>
       </c>
     </row>
-    <row r="22" spans="2:46" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:46" x14ac:dyDescent="0.35">
       <c r="B22">
         <v>43.480640049999998</v>
       </c>
@@ -5292,7 +5292,7 @@
         <v>43.480640049999998</v>
       </c>
     </row>
-    <row r="23" spans="2:46" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:46" x14ac:dyDescent="0.35">
       <c r="B23">
         <v>42.595909290000002</v>
       </c>
@@ -5423,7 +5423,7 @@
         <v>42.595909290000002</v>
       </c>
     </row>
-    <row r="24" spans="2:46" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:46" x14ac:dyDescent="0.35">
       <c r="B24">
         <v>44.276580000000003</v>
       </c>
@@ -5554,7 +5554,7 @@
         <v>44.276580000000003</v>
       </c>
     </row>
-    <row r="25" spans="2:46" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:46" x14ac:dyDescent="0.35">
       <c r="B25">
         <v>44.329900000000002</v>
       </c>
@@ -5685,7 +5685,7 @@
         <v>44.329900000000002</v>
       </c>
     </row>
-    <row r="26" spans="2:46" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:46" x14ac:dyDescent="0.35">
       <c r="B26">
         <v>42.186900000000001</v>
       </c>
@@ -5813,7 +5813,7 @@
         <v>42.186900000000001</v>
       </c>
     </row>
-    <row r="27" spans="2:46" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:46" x14ac:dyDescent="0.35">
       <c r="B27">
         <v>42.206899999999997</v>
       </c>
@@ -5944,7 +5944,7 @@
         <v>42.206899999999997</v>
       </c>
     </row>
-    <row r="28" spans="2:46" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:46" x14ac:dyDescent="0.35">
       <c r="B28">
         <v>42.448703299999998</v>
       </c>
@@ -6075,7 +6075,7 @@
         <v>42.448703299999998</v>
       </c>
     </row>
-    <row r="29" spans="2:46" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:46" x14ac:dyDescent="0.35">
       <c r="B29">
         <v>42.878349999999998</v>
       </c>
@@ -6203,7 +6203,7 @@
         <v>42.878349999999998</v>
       </c>
     </row>
-    <row r="30" spans="2:46" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:46" x14ac:dyDescent="0.35">
       <c r="B30">
         <v>42.880051999999999</v>
       </c>
@@ -6331,7 +6331,7 @@
         <v>42.880051999999999</v>
       </c>
     </row>
-    <row r="31" spans="2:46" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:46" x14ac:dyDescent="0.35">
       <c r="B31">
         <v>43.109648149999998</v>
       </c>
@@ -6459,7 +6459,7 @@
         <v>43.109648149999998</v>
       </c>
     </row>
-    <row r="32" spans="2:46" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:46" x14ac:dyDescent="0.35">
       <c r="B32">
         <v>42.461820000000003</v>
       </c>
@@ -6590,7 +6590,7 @@
         <v>42.461820000000003</v>
       </c>
     </row>
-    <row r="33" spans="2:46" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:46" x14ac:dyDescent="0.35">
       <c r="B33">
         <v>42.34695</v>
       </c>
@@ -6718,7 +6718,7 @@
         <v>42.34695</v>
       </c>
     </row>
-    <row r="34" spans="2:46" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:46" x14ac:dyDescent="0.35">
       <c r="B34">
         <v>42.49044</v>
       </c>
@@ -6846,7 +6846,7 @@
         <v>42.49044</v>
       </c>
     </row>
-    <row r="35" spans="2:46" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:46" x14ac:dyDescent="0.35">
       <c r="B35">
         <v>42.663980000000002</v>
       </c>
@@ -6974,7 +6974,7 @@
         <v>42.663980000000002</v>
       </c>
     </row>
-    <row r="36" spans="2:46" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:46" x14ac:dyDescent="0.35">
       <c r="B36">
         <v>41.958831000000004</v>
       </c>
@@ -7105,7 +7105,7 @@
         <v>41.958831000000004</v>
       </c>
     </row>
-    <row r="37" spans="2:46" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:46" x14ac:dyDescent="0.35">
       <c r="B37">
         <v>42.650626000000003</v>
       </c>
@@ -7242,7 +7242,7 @@
         <v>42.650626000000003</v>
       </c>
     </row>
-    <row r="38" spans="2:46" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:46" x14ac:dyDescent="0.35">
       <c r="B38">
         <v>42.676699999999997</v>
       </c>
@@ -7379,7 +7379,7 @@
         <v>42.676699999999997</v>
       </c>
     </row>
-    <row r="39" spans="2:46" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:46" x14ac:dyDescent="0.35">
       <c r="B39">
         <v>42.651211000000004</v>
       </c>
@@ -7516,7 +7516,7 @@
         <v>42.651211000000004</v>
       </c>
     </row>
-    <row r="40" spans="2:46" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:46" x14ac:dyDescent="0.35">
       <c r="B40">
         <v>42.595067999999998</v>
       </c>
@@ -7632,7 +7632,7 @@
         <v>42.595067999999998</v>
       </c>
     </row>
-    <row r="41" spans="2:46" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:46" x14ac:dyDescent="0.35">
       <c r="B41">
         <v>42.558070999999998</v>
       </c>
@@ -7763,7 +7763,7 @@
         <v>42.558070999999998</v>
       </c>
     </row>
-    <row r="42" spans="2:46" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:46" x14ac:dyDescent="0.35">
       <c r="B42">
         <v>43.580278</v>
       </c>
@@ -7894,7 +7894,7 @@
         <v>43.580278</v>
       </c>
     </row>
-    <row r="43" spans="2:46" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:46" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B43" s="4">
         <v>42.994239999999998</v>
       </c>
@@ -7974,7 +7974,7 @@
         <v>42.994239999999998</v>
       </c>
     </row>
-    <row r="44" spans="2:46" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:46" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B44" s="4">
         <v>42.89506454</v>
       </c>
@@ -8054,7 +8054,7 @@
         <v>42.89506454</v>
       </c>
     </row>
-    <row r="45" spans="2:46" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:46" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B45" s="4">
         <v>43.041046710000003</v>
       </c>
@@ -8134,7 +8134,7 @@
         <v>43.041046710000003</v>
       </c>
     </row>
-    <row r="46" spans="2:46" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:46" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B46" s="4">
         <v>43.047820000000002</v>
       </c>
@@ -8214,7 +8214,7 @@
         <v>43.047820000000002</v>
       </c>
     </row>
-    <row r="47" spans="2:46" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:46" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B47" s="4">
         <v>43.518279999999997</v>
       </c>
@@ -8294,7 +8294,7 @@
         <v>43.518279999999997</v>
       </c>
     </row>
-    <row r="48" spans="2:46" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:46" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B48" s="4">
         <v>43.518279999999997</v>
       </c>
@@ -8374,7 +8374,7 @@
         <v>43.518279999999997</v>
       </c>
     </row>
-    <row r="49" spans="2:46" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:46" x14ac:dyDescent="0.35">
       <c r="B49">
         <v>41.120049999999999</v>
       </c>
@@ -8508,7 +8508,7 @@
         <v>41.120049999999999</v>
       </c>
     </row>
-    <row r="50" spans="2:46" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:46" x14ac:dyDescent="0.35">
       <c r="B50">
         <v>41.202672999999997</v>
       </c>
@@ -8642,7 +8642,7 @@
         <v>41.202672999999997</v>
       </c>
     </row>
-    <row r="51" spans="2:46" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:46" x14ac:dyDescent="0.35">
       <c r="B51">
         <v>41.067979999999999</v>
       </c>
@@ -8770,7 +8770,7 @@
         <v>41.067979999999999</v>
       </c>
     </row>
-    <row r="52" spans="2:46" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:46" x14ac:dyDescent="0.35">
       <c r="B52">
         <v>41.058869999999999</v>
       </c>
@@ -8904,7 +8904,7 @@
         <v>41.058869999999999</v>
       </c>
     </row>
-    <row r="53" spans="2:46" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:46" x14ac:dyDescent="0.35">
       <c r="B53">
         <v>41.179858000000003</v>
       </c>
@@ -9038,7 +9038,7 @@
         <v>41.179858000000003</v>
       </c>
     </row>
-    <row r="54" spans="2:46" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:46" x14ac:dyDescent="0.35">
       <c r="B54">
         <v>41.196339999999999</v>
       </c>
@@ -9172,7 +9172,7 @@
         <v>41.196339999999999</v>
       </c>
     </row>
-    <row r="55" spans="2:46" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:46" x14ac:dyDescent="0.35">
       <c r="B55">
         <v>41.227381999999999</v>
       </c>
@@ -9306,7 +9306,7 @@
         <v>41.227381999999999</v>
       </c>
     </row>
-    <row r="56" spans="2:46" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:46" x14ac:dyDescent="0.35">
       <c r="B56">
         <v>41.133870000000002</v>
       </c>
@@ -9437,7 +9437,7 @@
         <v>41.133870000000002</v>
       </c>
     </row>
-    <row r="57" spans="2:46" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:46" x14ac:dyDescent="0.35">
       <c r="B57">
         <v>41.048411000000002</v>
       </c>
@@ -9568,7 +9568,7 @@
         <v>41.048411000000002</v>
       </c>
     </row>
-    <row r="58" spans="2:46" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:46" x14ac:dyDescent="0.35">
       <c r="B58">
         <v>41.174750000000003</v>
       </c>
@@ -9702,7 +9702,7 @@
         <v>41.174750000000003</v>
       </c>
     </row>
-    <row r="59" spans="2:46" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:46" x14ac:dyDescent="0.35">
       <c r="B59">
         <v>4.0875700000000004</v>
       </c>
@@ -9836,7 +9836,7 @@
         <v>4.0875700000000004</v>
       </c>
     </row>
-    <row r="60" spans="2:46" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:46" x14ac:dyDescent="0.35">
       <c r="B60">
         <v>41.145919999999997</v>
       </c>
@@ -9970,7 +9970,7 @@
         <v>41.145919999999997</v>
       </c>
     </row>
-    <row r="61" spans="2:46" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:46" x14ac:dyDescent="0.35">
       <c r="B61">
         <v>41.045999999999999</v>
       </c>
@@ -10104,7 +10104,7 @@
         <v>41.045999999999999</v>
       </c>
     </row>
-    <row r="62" spans="2:46" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:46" x14ac:dyDescent="0.35">
       <c r="B62">
         <v>42.404339999999998</v>
       </c>
@@ -10235,7 +10235,7 @@
         <v>42.404339999999998</v>
       </c>
     </row>
-    <row r="63" spans="2:46" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:46" x14ac:dyDescent="0.35">
       <c r="B63">
         <v>42.413609999999998</v>
       </c>
@@ -10366,7 +10366,7 @@
         <v>42.413609999999998</v>
       </c>
     </row>
-    <row r="64" spans="2:46" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:46" x14ac:dyDescent="0.35">
       <c r="B64">
         <v>42.45749</v>
       </c>
@@ -10497,7 +10497,7 @@
         <v>42.45749</v>
       </c>
     </row>
-    <row r="65" spans="2:46" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:46" x14ac:dyDescent="0.35">
       <c r="B65">
         <v>42.466000000000001</v>
       </c>
@@ -10631,7 +10631,7 @@
         <v>42.466000000000001</v>
       </c>
     </row>
-    <row r="66" spans="2:46" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:46" x14ac:dyDescent="0.35">
       <c r="B66">
         <v>42.46602</v>
       </c>
@@ -10765,7 +10765,7 @@
         <v>42.46602</v>
       </c>
     </row>
-    <row r="67" spans="2:46" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:46" x14ac:dyDescent="0.35">
       <c r="B67">
         <v>42.047359999999998</v>
       </c>
@@ -10884,7 +10884,7 @@
         <v>42.047359999999998</v>
       </c>
     </row>
-    <row r="68" spans="2:46" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:46" x14ac:dyDescent="0.35">
       <c r="B68">
         <v>42.118899999999996</v>
       </c>
@@ -11009,7 +11009,7 @@
         <v>42.118899999999996</v>
       </c>
     </row>
-    <row r="69" spans="2:46" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:46" x14ac:dyDescent="0.35">
       <c r="B69">
         <v>42.615549999999999</v>
       </c>
@@ -11143,7 +11143,7 @@
         <v>42.615549999999999</v>
       </c>
     </row>
-    <row r="70" spans="2:46" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:46" x14ac:dyDescent="0.35">
       <c r="B70">
         <v>42.555473480000003</v>
       </c>
@@ -11281,19 +11281,19 @@
   <dimension ref="A1:R65"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="17.85546875" customWidth="1"/>
-    <col min="4" max="4" width="19.5703125" style="4" customWidth="1"/>
-    <col min="7" max="7" width="20.42578125" style="7" customWidth="1"/>
-    <col min="8" max="8" width="14.7109375" customWidth="1"/>
-    <col min="9" max="9" width="21.42578125" customWidth="1"/>
+    <col min="3" max="3" width="17.81640625" customWidth="1"/>
+    <col min="4" max="4" width="26.1796875" style="4" customWidth="1"/>
+    <col min="7" max="7" width="20.453125" style="7" customWidth="1"/>
+    <col min="8" max="8" width="14.7265625" customWidth="1"/>
+    <col min="9" max="9" width="21.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -11349,7 +11349,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>182</v>
       </c>
@@ -11402,7 +11402,7 @@
         <v>43.55321</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>207</v>
       </c>
@@ -11446,7 +11446,7 @@
         <v>43.000165780000003</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>208</v>
       </c>
@@ -11490,7 +11490,7 @@
         <v>43.043680000000002</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>209</v>
       </c>
@@ -11543,7 +11543,7 @@
         <v>43.219700000000003</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>210</v>
       </c>
@@ -11596,7 +11596,7 @@
         <v>43.314999999999998</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>211</v>
       </c>
@@ -11649,7 +11649,7 @@
         <v>43.348599999999998</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>212</v>
       </c>
@@ -11702,7 +11702,7 @@
         <v>41.958831099999998</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>213</v>
       </c>
@@ -11755,7 +11755,7 @@
         <v>42.683332999999998</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>214</v>
       </c>
@@ -11808,7 +11808,7 @@
         <v>42.65</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>215</v>
       </c>
@@ -11861,7 +11861,7 @@
         <v>42.65</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>216</v>
       </c>
@@ -11914,7 +11914,7 @@
         <v>42.433332999999998</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>217</v>
       </c>
@@ -11967,7 +11967,7 @@
         <v>42.516666999999998</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>218</v>
       </c>
@@ -12020,7 +12020,7 @@
         <v>44.310417000000001</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>219</v>
       </c>
@@ -12073,7 +12073,7 @@
         <v>42.206899999999997</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>220</v>
       </c>
@@ -12126,7 +12126,7 @@
         <v>42.596159999999998</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>221</v>
       </c>
@@ -12179,7 +12179,7 @@
         <v>42.451894000000003</v>
       </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>222</v>
       </c>
@@ -12229,7 +12229,7 @@
         <v>42.448320000000002</v>
       </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>223</v>
       </c>
@@ -12282,7 +12282,7 @@
         <v>42.650626000000003</v>
       </c>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>224</v>
       </c>
@@ -12335,7 +12335,7 @@
         <v>42.676699999999997</v>
       </c>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>225</v>
       </c>
@@ -12388,7 +12388,7 @@
         <v>41.2026732</v>
       </c>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>226</v>
       </c>
@@ -12441,7 +12441,7 @@
         <v>41.087569999999999</v>
       </c>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>227</v>
       </c>
@@ -12494,7 +12494,7 @@
         <v>42.651211000000004</v>
       </c>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>228</v>
       </c>
@@ -12547,7 +12547,7 @@
         <v>41.120049999999999</v>
       </c>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>229</v>
       </c>
@@ -12600,7 +12600,7 @@
         <v>41.045999999999999</v>
       </c>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>230</v>
       </c>
@@ -12653,7 +12653,7 @@
         <v>42.416310000000003</v>
       </c>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>231</v>
       </c>
@@ -12706,7 +12706,7 @@
         <v>41.048411000000002</v>
       </c>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>232</v>
       </c>
@@ -12759,7 +12759,7 @@
         <v>42.466000000000001</v>
       </c>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>233</v>
       </c>
@@ -12812,7 +12812,7 @@
         <v>41.133870000000002</v>
       </c>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>234</v>
       </c>
@@ -12865,7 +12865,7 @@
         <v>41.179858000000003</v>
       </c>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>235</v>
       </c>
@@ -12918,7 +12918,7 @@
         <v>42.047359999999998</v>
       </c>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>236</v>
       </c>
@@ -12971,7 +12971,7 @@
         <v>42.555619</v>
       </c>
     </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>237</v>
       </c>
@@ -13024,7 +13024,7 @@
         <v>41.058810000000001</v>
       </c>
     </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>238</v>
       </c>
@@ -13077,7 +13077,7 @@
         <v>42.118899999999996</v>
       </c>
     </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>239</v>
       </c>
@@ -13130,7 +13130,7 @@
         <v>42.404159999999997</v>
       </c>
     </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>240</v>
       </c>
@@ -13183,7 +13183,7 @@
         <v>41.227381999999999</v>
       </c>
     </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>241</v>
       </c>
@@ -13236,7 +13236,7 @@
         <v>41.067979999999999</v>
       </c>
     </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>242</v>
       </c>
@@ -13289,7 +13289,7 @@
         <v>42.46602</v>
       </c>
     </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>243</v>
       </c>
@@ -13342,7 +13342,7 @@
         <v>42.118899999999996</v>
       </c>
     </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>244</v>
       </c>
@@ -13395,7 +13395,7 @@
         <v>42.45749</v>
       </c>
     </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>245</v>
       </c>
@@ -13448,7 +13448,7 @@
         <v>43.696573999999998</v>
       </c>
     </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>246</v>
       </c>
@@ -13501,7 +13501,7 @@
         <v>42.613411999999997</v>
       </c>
     </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>247</v>
       </c>
@@ -13554,7 +13554,7 @@
         <v>44.276580000000003</v>
       </c>
     </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>248</v>
       </c>
@@ -13601,7 +13601,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>249</v>
       </c>
@@ -13654,7 +13654,7 @@
         <v>42.047359999999998</v>
       </c>
     </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>250</v>
       </c>
@@ -13707,7 +13707,7 @@
         <v>42.186929999999997</v>
       </c>
     </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>251</v>
       </c>
@@ -13760,7 +13760,7 @@
         <v>41.196339999999999</v>
       </c>
     </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>252</v>
       </c>
@@ -13807,7 +13807,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>253</v>
       </c>
@@ -13860,7 +13860,7 @@
         <v>42.116149999999998</v>
       </c>
     </row>
-    <row r="50" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>254</v>
       </c>
@@ -13913,7 +13913,7 @@
         <v>42.558070999999998</v>
       </c>
     </row>
-    <row r="51" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A51">
         <v>255</v>
       </c>
@@ -13966,7 +13966,7 @@
         <v>41.174750000000003</v>
       </c>
     </row>
-    <row r="52" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A52">
         <v>256</v>
       </c>
@@ -14019,7 +14019,7 @@
         <v>43.696570000000001</v>
       </c>
     </row>
-    <row r="53" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A53">
         <v>257</v>
       </c>
@@ -14072,7 +14072,7 @@
         <v>41.145420199999997</v>
       </c>
     </row>
-    <row r="54" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A54">
         <v>258</v>
       </c>
@@ -14125,7 +14125,7 @@
         <v>42.590679999999999</v>
       </c>
     </row>
-    <row r="55" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A55">
         <v>259</v>
       </c>
@@ -14178,7 +14178,7 @@
         <v>43.409284</v>
       </c>
     </row>
-    <row r="56" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A56">
         <v>260</v>
       </c>
@@ -14231,7 +14231,7 @@
         <v>42.626193000000001</v>
       </c>
     </row>
-    <row r="57" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A57">
         <v>261</v>
       </c>
@@ -14284,7 +14284,7 @@
         <v>43.417945000000003</v>
       </c>
     </row>
-    <row r="58" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A58">
         <v>262</v>
       </c>
@@ -14337,7 +14337,7 @@
         <v>43.480690000000003</v>
       </c>
     </row>
-    <row r="59" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A59">
         <v>263</v>
       </c>
@@ -14390,7 +14390,7 @@
         <v>43.580300000000001</v>
       </c>
     </row>
-    <row r="60" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A60">
         <v>264</v>
       </c>
@@ -14443,7 +14443,7 @@
         <v>43.636978999999997</v>
       </c>
     </row>
-    <row r="61" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A61">
         <v>265</v>
       </c>
@@ -14496,7 +14496,7 @@
         <v>43.4159942</v>
       </c>
     </row>
-    <row r="62" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A62">
         <v>266</v>
       </c>
@@ -14549,7 +14549,7 @@
         <v>43.518279999999997</v>
       </c>
     </row>
-    <row r="63" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A63">
         <v>267</v>
       </c>
@@ -14602,7 +14602,7 @@
         <v>43.518279999999997</v>
       </c>
     </row>
-    <row r="64" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A64">
         <v>268</v>
       </c>
@@ -14655,7 +14655,7 @@
         <v>43.480739999999997</v>
       </c>
     </row>
-    <row r="65" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A65">
         <v>269</v>
       </c>

</xml_diff>